<commit_message>
ready backend and add upload, need add carousel
</commit_message>
<xml_diff>
--- a/display/kiosk_bot/server/upload/sch_pn.xlsx
+++ b/display/kiosk_bot/server/upload/sch_pn.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curvh\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="sch"/>
+    <sheet name="sch" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_5А" localSheetId="0">sch!$B$2:$B$8</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -85,9 +90,6 @@
     <t>11А</t>
   </si>
   <si>
-    <t>здарова</t>
-  </si>
-  <si>
     <t>Толмачева</t>
   </si>
   <si>
@@ -275,13 +277,15 @@
   </si>
   <si>
     <t>2.7</t>
+  </si>
+  <si>
+    <t>привет</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,13 +302,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFc00000"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -326,6 +324,12 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,85 +502,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -587,10 +590,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -628,71 +631,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -720,7 +723,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -743,11 +746,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -756,13 +759,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -772,7 +775,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -781,7 +784,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -790,7 +793,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -798,10 +801,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -872,77 +875,17 @@
   </sheetPr>
   <dimension ref="A1:BL20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="64" width="13.5703125" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1136,29 +1079,29 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
+    <row r="2" spans="1:64" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -1186,97 +1129,97 @@
       <c r="AG2" s="8"/>
       <c r="AH2" s="8"/>
       <c r="AI2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK2" s="8"/>
       <c r="AL2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AM2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN2" s="8"/>
       <c r="AO2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AP2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AQ2" s="8"/>
       <c r="AR2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AS2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AT2" s="8"/>
       <c r="AU2" s="6"/>
       <c r="AV2" s="8"/>
       <c r="AW2" s="8"/>
       <c r="AX2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AY2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AZ2" s="8"/>
       <c r="BA2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="BB2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="BC2" s="8"/>
       <c r="BD2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="BE2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BF2" s="8"/>
       <c r="BG2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="BH2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BI2" s="8"/>
       <c r="BJ2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="BK2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BL2" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1304,97 +1247,97 @@
       <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
       <c r="AI3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="AK3" s="8"/>
       <c r="AL3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AN3" s="8"/>
       <c r="AO3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP3" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="AP3" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="AQ3" s="8"/>
       <c r="AR3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AS3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AT3" s="8"/>
       <c r="AU3" s="10"/>
       <c r="AV3" s="8"/>
       <c r="AW3" s="8"/>
       <c r="AX3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY3" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="AY3" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="AZ3" s="8"/>
       <c r="BA3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="BB3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BC3" s="8"/>
       <c r="BD3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE3" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="BE3" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="BF3" s="8"/>
       <c r="BG3" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BH3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI3" s="8"/>
       <c r="BJ3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BK3" s="7" t="s">
+      <c r="BL3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BL3" s="7" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -1422,99 +1365,99 @@
       <c r="AG4" s="8"/>
       <c r="AH4" s="8"/>
       <c r="AI4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AK4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AK4" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="AL4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AM4" s="7" t="s">
+      <c r="AN4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AN4" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="AO4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AP4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ4" s="8"/>
       <c r="AR4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AT4" s="8"/>
       <c r="AU4" s="10"/>
       <c r="AV4" s="8"/>
       <c r="AW4" s="8"/>
       <c r="AX4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AZ4" s="8"/>
       <c r="BA4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BB4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="BC4" s="8"/>
       <c r="BD4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE4" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="BE4" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="BF4" s="8"/>
       <c r="BG4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="BH4" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="BH4" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="BI4" s="8"/>
       <c r="BJ4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BK4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BL4" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -1542,95 +1485,95 @@
       <c r="AG5" s="8"/>
       <c r="AH5" s="8"/>
       <c r="AI5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AJ5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK5" s="8"/>
       <c r="AL5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM5" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="AM5" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="AN5" s="8"/>
       <c r="AO5" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AQ5" s="8"/>
       <c r="AR5" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AT5" s="8"/>
       <c r="AU5" s="10"/>
       <c r="AV5" s="8"/>
       <c r="AW5" s="8"/>
       <c r="AX5" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AY5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AZ5" s="8"/>
       <c r="BA5" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BB5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BC5" s="8"/>
       <c r="BD5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BE5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BF5" s="8"/>
       <c r="BG5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BH5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BI5" s="8"/>
       <c r="BJ5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="BK5" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="BK5" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="BL5" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1658,97 +1601,97 @@
       <c r="AG6" s="8"/>
       <c r="AH6" s="8"/>
       <c r="AI6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AJ6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AK6" s="8"/>
       <c r="AL6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AN6" s="8"/>
       <c r="AO6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AQ6" s="8"/>
       <c r="AR6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AS6" s="7" t="s">
+      <c r="AT6" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="AT6" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="AU6" s="10"/>
       <c r="AV6" s="8"/>
       <c r="AW6" s="8"/>
       <c r="AX6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AY6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AZ6" s="8"/>
       <c r="BA6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB6" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="BB6" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="BC6" s="8"/>
       <c r="BD6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BE6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BF6" s="8"/>
       <c r="BG6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH6" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="BH6" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="BI6" s="8"/>
       <c r="BJ6" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BK6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BL6" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1776,90 +1719,90 @@
       <c r="AG7" s="8"/>
       <c r="AH7" s="8"/>
       <c r="AI7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="AJ7" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="AK7" s="8"/>
       <c r="AL7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AM7" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AN7" s="8"/>
       <c r="AO7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AQ7" s="8"/>
       <c r="AR7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AS7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AT7" s="8"/>
       <c r="AU7" s="10"/>
       <c r="AV7" s="8"/>
       <c r="AW7" s="8"/>
       <c r="AX7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AY7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AZ7" s="8"/>
       <c r="BA7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="BB7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="BC7" s="8"/>
       <c r="BD7" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BE7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BF7" s="8"/>
       <c r="BG7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH7" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="BH7" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="BI7" s="8"/>
       <c r="BJ7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BK7" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="BL7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>67</v>
+      <c r="B8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="13" t="s">
-        <v>67</v>
+      <c r="E8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="13" t="s">
-        <v>67</v>
+      <c r="H8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -1887,190 +1830,190 @@
       <c r="AF8" s="8"/>
       <c r="AG8" s="8"/>
       <c r="AH8" s="8"/>
-      <c r="AI8" s="14"/>
+      <c r="AI8" s="13"/>
       <c r="AJ8" s="8"/>
       <c r="AK8" s="8"/>
       <c r="AL8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN8" s="8"/>
       <c r="AO8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AP8" s="7" t="s">
+      <c r="AQ8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AQ8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR8" s="14" t="s">
-        <v>42</v>
+      <c r="AR8" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="AS8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AT8" s="8"/>
       <c r="AU8" s="10"/>
       <c r="AV8" s="8"/>
       <c r="AW8" s="8"/>
-      <c r="AX8" s="15" t="s">
+      <c r="AX8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY8" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="AY8" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="AZ8" s="8"/>
       <c r="BA8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB8" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="BB8" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="BC8" s="8"/>
       <c r="BD8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BE8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BF8" s="8"/>
       <c r="BG8" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BH8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BI8" s="8"/>
       <c r="BJ8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BL8" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>67</v>
+    <row r="9" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="17" t="s">
-        <v>67</v>
+      <c r="E9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="17" t="s">
-        <v>67</v>
+      <c r="H9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
       <c r="T9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y9" s="8"/>
       <c r="Z9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AA9" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB9" s="8"/>
       <c r="AC9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AD9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE9" s="8"/>
       <c r="AF9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AG9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH9" s="8"/>
-      <c r="AI9" s="17" t="s">
-        <v>67</v>
+      <c r="AI9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AJ9" s="8"/>
       <c r="AK9" s="8"/>
-      <c r="AL9" s="17"/>
+      <c r="AL9" s="16"/>
       <c r="AM9" s="8"/>
       <c r="AN9" s="8"/>
-      <c r="AO9" s="17"/>
+      <c r="AO9" s="16"/>
       <c r="AP9" s="8"/>
       <c r="AQ9" s="8"/>
-      <c r="AR9" s="17" t="s">
-        <v>67</v>
+      <c r="AR9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AS9" s="8"/>
       <c r="AT9" s="8"/>
-      <c r="AU9" s="17"/>
+      <c r="AU9" s="16"/>
       <c r="AV9" s="8"/>
       <c r="AW9" s="8"/>
-      <c r="AX9" s="17" t="s">
-        <v>67</v>
+      <c r="AX9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AY9" s="8"/>
       <c r="AZ9" s="8"/>
-      <c r="BA9" s="17" t="s">
-        <v>67</v>
+      <c r="BA9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="BB9" s="8"/>
       <c r="BC9" s="8"/>
-      <c r="BD9" s="17" t="s">
-        <v>67</v>
+      <c r="BD9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="BE9" s="8"/>
       <c r="BF9" s="8"/>
       <c r="BG9" s="10"/>
       <c r="BH9" s="8"/>
       <c r="BI9" s="8"/>
-      <c r="BJ9" s="17" t="s">
-        <v>67</v>
+      <c r="BJ9" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="BK9" s="8"/>
       <c r="BL9" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="18" t="s">
-        <v>72</v>
+    <row r="10" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2082,62 +2025,62 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V10" s="8"/>
       <c r="W10" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y10" s="8"/>
       <c r="Z10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB10" s="8"/>
       <c r="AC10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE10" s="8"/>
       <c r="AF10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AH10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8"/>
@@ -2170,9 +2113,9 @@
       <c r="BK10" s="8"/>
       <c r="BL10" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="18" t="s">
-        <v>76</v>
+    <row r="11" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2184,59 +2127,59 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S11" s="8"/>
       <c r="T11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="U11" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="U11" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y11" s="8"/>
       <c r="Z11" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE11" s="8"/>
       <c r="AF11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG11" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="AG11" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="AH11" s="8"/>
       <c r="AI11" s="8"/>
@@ -2270,9 +2213,9 @@
       <c r="BK11" s="8"/>
       <c r="BL11" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="19" t="s">
-        <v>77</v>
+    <row r="12" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>76</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2284,59 +2227,59 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="R12" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="S12" s="8"/>
       <c r="T12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U12" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="V12" s="8"/>
       <c r="W12" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y12" s="8"/>
       <c r="Z12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA12" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="AA12" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AE12" s="8"/>
       <c r="AF12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AG12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH12" s="8"/>
       <c r="AI12" s="8"/>
@@ -2370,9 +2313,9 @@
       <c r="BK12" s="8"/>
       <c r="BL12" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="16" t="s">
-        <v>80</v>
+    <row r="13" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2384,61 +2327,61 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="R13" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="S13" s="8"/>
       <c r="T13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="V13" s="8"/>
       <c r="W13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB13" s="8"/>
       <c r="AC13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD13" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="AD13" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="AE13" s="8"/>
       <c r="AF13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH13" s="8"/>
       <c r="AI13" s="8"/>
@@ -2472,9 +2415,9 @@
       <c r="BK13" s="8"/>
       <c r="BL13" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="16" t="s">
-        <v>81</v>
+    <row r="14" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2486,61 +2429,61 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S14" s="8"/>
       <c r="T14" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V14" s="8"/>
       <c r="W14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y14" s="8"/>
       <c r="Z14" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AA14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD14" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="AD14" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="AE14" s="8"/>
       <c r="AF14" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH14" s="8"/>
       <c r="AI14" s="8"/>
@@ -2574,9 +2517,9 @@
       <c r="BK14" s="8"/>
       <c r="BL14" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="16" t="s">
-        <v>82</v>
+    <row r="15" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2588,59 +2531,59 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R15" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="S15" s="8"/>
       <c r="T15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="V15" s="8"/>
+      <c r="W15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="U15" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="V15" s="8"/>
-      <c r="W15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="X15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="15" t="s">
-        <v>79</v>
-      </c>
       <c r="AA15" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB15" s="8"/>
       <c r="AC15" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AD15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE15" s="8"/>
       <c r="AF15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG15" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="AG15" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="AH15" s="8"/>
       <c r="AI15" s="8"/>
@@ -2674,9 +2617,9 @@
       <c r="BK15" s="8"/>
       <c r="BL15" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="16" t="s">
-        <v>85</v>
+    <row r="16" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2687,43 +2630,43 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="15" t="s">
-        <v>67</v>
+      <c r="K16" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="15" t="s">
-        <v>67</v>
+      <c r="N16" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="14" t="s">
-        <v>67</v>
+      <c r="Q16" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
-      <c r="T16" s="14" t="s">
-        <v>67</v>
+      <c r="T16" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
-      <c r="W16" s="14" t="s">
-        <v>67</v>
+      <c r="W16" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
-      <c r="Z16" s="15" t="s">
-        <v>67</v>
+      <c r="Z16" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
-      <c r="AC16" s="15" t="s">
-        <v>67</v>
+      <c r="AC16" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
-      <c r="AF16" s="20" t="s">
-        <v>67</v>
+      <c r="AF16" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
@@ -2758,7 +2701,7 @@
       <c r="BK16" s="8"/>
       <c r="BL16" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2769,42 +2712,42 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="17" t="s">
-        <v>67</v>
+      <c r="K17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="17" t="s">
-        <v>67</v>
+      <c r="N17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="17" t="s">
-        <v>67</v>
+      <c r="Q17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="17" t="s">
-        <v>67</v>
+      <c r="T17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
-      <c r="W17" s="17" t="s">
-        <v>67</v>
+      <c r="W17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
-      <c r="Z17" s="17" t="s">
-        <v>67</v>
+      <c r="Z17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
-      <c r="AC17" s="17" t="s">
-        <v>67</v>
+      <c r="AC17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AD17" s="8"/>
-      <c r="AE17" s="17" t="s">
-        <v>67</v>
+      <c r="AE17" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
@@ -2840,8 +2783,8 @@
       <c r="BK17" s="8"/>
       <c r="BL17" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="21"/>
+    <row r="18" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2906,8 +2849,8 @@
       <c r="BK18" s="8"/>
       <c r="BL18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="16"/>
+    <row r="19" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2972,8 +2915,8 @@
       <c r="BK19" s="8"/>
       <c r="BL19" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>

</xml_diff>